<commit_message>
Waardelijst voor Reflevel toegevoegd
</commit_message>
<xml_diff>
--- a/BROCategoricals/Waardelijsten BRO GLD.xlsx
+++ b/BROCategoricals/Waardelijsten BRO GLD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://3hydro-my.sharepoint.com/personal/jos_von_asmuth_3hydro_nl/Documents/MATLAB/Menyanthes/Meny_OS/trunk/Datamodels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\RWS Ketentest\pybron\BronDatamodel\BROCategoricals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD75B709-8905-47E5-8321-2446D97594E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB63FF50-C301-41CD-B975-70008C5C0C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="28800" windowHeight="15372" xr2:uid="{9B78218B-74B7-49DD-AC23-EE4FE51EA6CA}"/>
+    <workbookView xWindow="33240" yWindow="2895" windowWidth="24120" windowHeight="12060" firstSheet="7" activeTab="11" xr2:uid="{9B78218B-74B7-49DD-AC23-EE4FE51EA6CA}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusQualityControl" sheetId="12" r:id="rId1"/>
@@ -24,18 +24,30 @@
     <sheet name="CorrectionReason" sheetId="4" r:id="rId9"/>
     <sheet name="CensoredReason" sheetId="3" r:id="rId10"/>
     <sheet name="AirPressureCompensationType" sheetId="2" r:id="rId11"/>
+    <sheet name="RefLevel" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="110">
   <si>
     <t>Codes</t>
   </si>
@@ -359,6 +371,12 @@
   </si>
   <si>
     <t>Er zijn twijfels over de juistheid van dit gegeven, maar uitsluitsel kon niet gegeven worden op basis van de gehanteerde beoordelingsprocedure.</t>
+  </si>
+  <si>
+    <t>NAP</t>
+  </si>
+  <si>
+    <t>Referentie voor hoogtemetingen</t>
   </si>
 </sst>
 </file>
@@ -571,7 +589,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -587,7 +605,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -885,15 +903,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5218D3DD-5DEE-42B7-A314-1FFE98200F27}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -907,7 +925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -921,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>99</v>
       </c>
@@ -935,7 +953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>101</v>
       </c>
@@ -949,7 +967,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>103</v>
       </c>
@@ -963,7 +981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -977,7 +995,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>106</v>
       </c>
@@ -1000,15 +1018,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44556876-1C9C-4067-A49D-EEE4928A668A}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1036,7 +1056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
@@ -1050,7 +1070,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
@@ -1089,13 +1109,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1123,7 +1143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1137,7 +1157,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1151,7 +1171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1185,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1179,7 +1199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1193,7 +1213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
@@ -1205,6 +1225,66 @@
       </c>
       <c r="D8" s="12" t="s">
         <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D01BD6-872E-42EA-ABB8-8E8EFB77A528}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1218,13 +1298,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1252,7 +1332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -1266,7 +1346,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>95</v>
       </c>
@@ -1280,7 +1360,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>97</v>
       </c>
@@ -1305,13 +1385,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>92</v>
       </c>
@@ -1364,13 +1444,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1398,7 +1478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>75</v>
       </c>
@@ -1412,7 +1492,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>77</v>
       </c>
@@ -1426,7 +1506,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>79</v>
       </c>
@@ -1440,7 +1520,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>81</v>
       </c>
@@ -1454,7 +1534,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>83</v>
       </c>
@@ -1468,7 +1548,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>85</v>
       </c>
@@ -1482,7 +1562,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1496,7 +1576,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>88</v>
       </c>
@@ -1510,7 +1590,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>90</v>
       </c>
@@ -1535,13 +1615,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1569,7 +1649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>71</v>
       </c>
@@ -1583,7 +1663,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>73</v>
       </c>
@@ -1608,13 +1688,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,7 +1708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1642,7 +1722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>52</v>
       </c>
@@ -1656,7 +1736,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
@@ -1670,7 +1750,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>56</v>
       </c>
@@ -1684,7 +1764,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>58</v>
       </c>
@@ -1698,7 +1778,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>60</v>
       </c>
@@ -1712,7 +1792,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1726,7 +1806,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>63</v>
       </c>
@@ -1740,7 +1820,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>65</v>
       </c>
@@ -1754,7 +1834,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>67</v>
       </c>
@@ -1768,7 +1848,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>69</v>
       </c>
@@ -1793,13 +1873,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1813,7 +1893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1827,7 +1907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>50</v>
       </c>
@@ -1852,13 +1932,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1886,7 +1966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
@@ -1900,7 +1980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
@@ -1914,7 +1994,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1928,7 +2008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
@@ -1942,7 +2022,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
@@ -1956,7 +2036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>40</v>
       </c>
@@ -1970,7 +2050,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -1984,7 +2064,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>44</v>
       </c>
@@ -1998,7 +2078,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
@@ -2012,7 +2092,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>48</v>
       </c>
@@ -2037,13 +2117,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2071,7 +2151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -2085,7 +2165,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
@@ -2099,7 +2179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
@@ -2113,7 +2193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>29</v>
       </c>

</xml_diff>